<commit_message>
Refactor user maintenance component to include user role in table display
</commit_message>
<xml_diff>
--- a/frontend/src/assets/users.xlsx
+++ b/frontend/src/assets/users.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -30,6 +30,9 @@
     <t>identification</t>
   </si>
   <si>
+    <t>role</t>
+  </si>
+  <si>
     <t>JuanAlberto1</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
   </si>
   <si>
     <t>Pass1234#</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -611,28 +617,34 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>1122334455</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>